<commit_message>
add case about show table distributions
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/mysqlcases/dql/casegroup1/mysql_dql_cases1.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/mysqlcases/dql/casegroup1/mysql_dql_cases1.xlsx
@@ -18931,8 +18931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1606"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1048" workbookViewId="0">
-      <selection activeCell="G1069" sqref="G1069"/>
+    <sheetView tabSelected="1" topLeftCell="A1489" workbookViewId="0">
+      <selection activeCell="C1501" sqref="C1501"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -60417,7 +60417,7 @@
         <v>4168</v>
       </c>
       <c r="B1501" s="4" t="s">
-        <v>34</v>
+        <v>4547</v>
       </c>
       <c r="C1501" s="1" t="s">
         <v>2609</v>

</xml_diff>

<commit_message>
add case about explain out
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/mysqlcases/dql/casegroup1/mysql_dql_cases1.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/mysqlcases/dql/casegroup1/mysql_dql_cases1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13902" uniqueCount="5249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13928" uniqueCount="5267">
   <si>
     <t>TestID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -18556,6 +18556,75 @@
   <si>
     <t>select char_length(left(current_timestamp,19))</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1606</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主键顺序和建表列顺序不一致的多分区表第一个主键范围查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RangeScan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>partition49</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>value_partition49</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $partition49 where name between 'Ww' and 'mp'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1607</t>
+  </si>
+  <si>
+    <t>主键顺序和建表列顺序不一致的多分区表第二个主键范围查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $partition49 where id between 49 and 5000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/mysqlcases/dql/casegroup1/expectedresult/RangeScan/queryc1_1606.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/mysqlcases/dql/casegroup1/expectedresult/RangeScan/queryc1_1607.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dqlc1_1608</t>
+  </si>
+  <si>
+    <t>explain输出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Explain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>schema17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qc1_value20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>explain plan for select * from $schema17 where id=2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>justExec</t>
   </si>
 </sst>
 </file>
@@ -18929,10 +18998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1606"/>
+  <dimension ref="A1:K1609"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1589" sqref="C1589"/>
+    <sheetView tabSelected="1" topLeftCell="A1587" workbookViewId="0">
+      <selection activeCell="H1609" sqref="H1609"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -63876,6 +63945,90 @@
         <v>44</v>
       </c>
     </row>
+    <row r="1607" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1607" s="1" t="s">
+        <v>5249</v>
+      </c>
+      <c r="B1607" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1607" s="1" t="s">
+        <v>5250</v>
+      </c>
+      <c r="D1607" s="1" t="s">
+        <v>5251</v>
+      </c>
+      <c r="F1607" s="1" t="s">
+        <v>5252</v>
+      </c>
+      <c r="G1607" s="1" t="s">
+        <v>5253</v>
+      </c>
+      <c r="I1607" s="1" t="s">
+        <v>5254</v>
+      </c>
+      <c r="J1607" s="1" t="s">
+        <v>5258</v>
+      </c>
+      <c r="K1607" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1608" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1608" s="1" t="s">
+        <v>5255</v>
+      </c>
+      <c r="B1608" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1608" s="1" t="s">
+        <v>5256</v>
+      </c>
+      <c r="D1608" s="1" t="s">
+        <v>5251</v>
+      </c>
+      <c r="F1608" s="1" t="s">
+        <v>5252</v>
+      </c>
+      <c r="H1608" s="1" t="s">
+        <v>5249</v>
+      </c>
+      <c r="I1608" s="1" t="s">
+        <v>5257</v>
+      </c>
+      <c r="J1608" s="1" t="s">
+        <v>5259</v>
+      </c>
+      <c r="K1608" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1609" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A1609" s="1" t="s">
+        <v>5260</v>
+      </c>
+      <c r="B1609" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1609" s="1" t="s">
+        <v>5261</v>
+      </c>
+      <c r="D1609" s="1" t="s">
+        <v>5262</v>
+      </c>
+      <c r="F1609" s="1" t="s">
+        <v>5263</v>
+      </c>
+      <c r="G1609" s="1" t="s">
+        <v>5264</v>
+      </c>
+      <c r="I1609" s="1" t="s">
+        <v>5265</v>
+      </c>
+      <c r="K1609" s="1" t="s">
+        <v>5266</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
@@ -63883,7 +64036,7 @@
       <formula1>"y,n"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576">
-      <formula1>"csv_equals,csv_containsAll,string_equals,double_equals,assertNull,SQLException"</formula1>
+      <formula1>"csv_equals,csv_containsAll,string_equals,double_equals,assertNull,justExec,SQLException"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add cases about mysql protocol
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/mysqlcases/dql/casegroup1/mysql_dql_cases1.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/mysqlcases/dql/casegroup1/mysql_dql_cases1.xlsx
@@ -19000,8 +19000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1609"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1587" workbookViewId="0">
-      <selection activeCell="H1609" sqref="H1609"/>
+    <sheetView tabSelected="1" topLeftCell="A1578" workbookViewId="0">
+      <selection activeCell="E1621" sqref="E1621"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
expected value updated as of float support
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/mysqlcases/dql/casegroup1/mysql_dql_cases1.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/mysqlcases/dql/casegroup1/mysql_dql_cases1.xlsx
@@ -19041,8 +19041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1610"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1577" workbookViewId="0">
-      <selection activeCell="C1613" sqref="C1613"/>
+    <sheetView tabSelected="1" topLeftCell="A1448" workbookViewId="0">
+      <selection activeCell="C1455" sqref="C1455"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>